<commit_message>
going througher almost done
</commit_message>
<xml_diff>
--- a/Dan_Project.xlsx
+++ b/Dan_Project.xlsx
@@ -92,9 +92,6 @@
     <t>Pair Programming</t>
   </si>
   <si>
-    <t>Token Stack complete</t>
-  </si>
-  <si>
     <t>Pushed everything and popped everything</t>
   </si>
   <si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>CLion, cmake, clang</t>
+  </si>
+  <si>
+    <t>Token Stack complete; Compiles on all</t>
   </si>
 </sst>
 </file>
@@ -447,7 +447,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -512,7 +512,7 @@
         <v>13</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="13" x14ac:dyDescent="0.15">
@@ -529,7 +529,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -540,16 +540,16 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>22</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Negs and Parentheses done
</commit_message>
<xml_diff>
--- a/Dan_Project.xlsx
+++ b/Dan_Project.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -105,6 +105,24 @@
   </si>
   <si>
     <t>Token Stack complete; Compiles on all</t>
+  </si>
+  <si>
+    <t>Feb 15th</t>
+  </si>
+  <si>
+    <t>Parentheses Not handled correctly</t>
+  </si>
+  <si>
+    <t>Clion, cmake, clang, gcc</t>
+  </si>
+  <si>
+    <t>Parentheses and Neg integers done</t>
+  </si>
+  <si>
+    <t>Testing with different inputs</t>
+  </si>
+  <si>
+    <t>Not correctly incrementing through string</t>
   </si>
 </sst>
 </file>
@@ -444,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -552,6 +570,34 @@
         <v>22</v>
       </c>
     </row>
+    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Dan's proj form
</commit_message>
<xml_diff>
--- a/Dan_Project.xlsx
+++ b/Dan_Project.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -138,6 +138,18 @@
   </si>
   <si>
     <t>Not correctly handling negative numbers or multi-digit integers.</t>
+  </si>
+  <si>
+    <t>dcstarne</t>
+  </si>
+  <si>
+    <t>Preassessment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gcc </t>
+  </si>
+  <si>
+    <t>Execute: ./main input.txt output.txt</t>
   </si>
 </sst>
 </file>
@@ -477,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -630,6 +642,23 @@
         <v>35</v>
       </c>
     </row>
+    <row r="17" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17">
+        <v>20170217</v>
+      </c>
+      <c r="B17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>